<commit_message>
added y-axis caption to diagrams
</commit_message>
<xml_diff>
--- a/diagrams/SeitenaufrufeTeamSports.xlsx
+++ b/diagrams/SeitenaufrufeTeamSports.xlsx
@@ -8,14 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiaskoenig/Projects/bachelor-thesis/mk-bachelor-thesis/diagrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEFFCE28-F6DB-2D49-AF30-CDC90793277A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CE1D7A-122A-7649-9DF4-3F80B1A9CBDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="640" windowWidth="27680" windowHeight="16880" xr2:uid="{9C9F30AC-90E1-4E3B-9DFE-54DBA87CD2E2}"/>
+    <workbookView xWindow="29260" yWindow="-11180" windowWidth="37560" windowHeight="20440" activeTab="1" xr2:uid="{9C9F30AC-90E1-4E3B-9DFE-54DBA87CD2E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Tabelle1!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Tabelle1!$B$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Tabelle2!$A$20:$A$31</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Tabelle2!$B$19</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Tabelle2!$B$20:$B$31</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Tabelle1!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Tabelle1!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Tabelle1!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Tabelle1!$B$2:$B$8</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Tabelle2!$A$3:$A$9</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Tabelle2!$B$3:$B$9</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">Tabelle2!$B$20:$B$31</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">Tabelle2!$A$20:$A$31</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">Tabelle2!$B$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>April</t>
   </si>
@@ -829,6 +845,673 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Seitenaufrufe im Wochenverlauf</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle2!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Montag</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dienstag</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mittwoch</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Donnerstag</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Freitag</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Samstag</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sonntag</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>90880</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45080</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105680</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105680</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EDE5-374B-8312-6C8CBB316C15}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1941986224"/>
+        <c:axId val="1920952976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1941986224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1920952976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1920952976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1941986224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Seitenaufrufe im Jahresverlauf</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle2!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Seitenaufrufe im Jahresverlauf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle2!$A$20:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Januar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Februar</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>März</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Juni</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Juli</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oktober</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dezember</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$B$20:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1267520</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1014880</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1856320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2503520</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3113600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>950000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>950000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1923210</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3148320</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3160320</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2663520</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2056320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A13-2548-8314-F4BE419E3248}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1924675760"/>
+        <c:axId val="1925133424"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1924675760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1925133424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1925133424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1924675760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="21">
   <a:schemeClr val="accent1"/>
@@ -875,6 +1558,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="103">
   <cs:axisTitle>
@@ -1779,6 +2542,1038 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx2"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1840,6 +3635,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFF5CDC8-1215-4930-B3A3-D1520C98BDC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{277DE0D4-81CC-EF4B-A293-0BB171A1195A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>621030</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>167386</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6304353B-8769-5F4A-8ABF-EF2AA86F9CFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2159,8 +4031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF2F794-32EC-4398-97C0-77FCA5D72016}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2345,14 +4217,220 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927D0A81-5441-438F-B462-CE72DE2868CA}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>90880</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>62720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>53080</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>45080</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>70240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>105680</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>105680</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>1267520</v>
+      </c>
+      <c r="C20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>1014880</v>
+      </c>
+      <c r="C21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>1856320</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>2503520</v>
+      </c>
+      <c r="C23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24">
+        <v>3113600</v>
+      </c>
+      <c r="C24">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <v>950000</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <v>950000</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1923210</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>3148320</v>
+      </c>
+      <c r="C28">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>3160320</v>
+      </c>
+      <c r="C29">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>2663520</v>
+      </c>
+      <c r="C30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>2056320</v>
+      </c>
+      <c r="C31">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>